<commit_message>
Datasheet added to info folder
</commit_message>
<xml_diff>
--- a/Project walkthrough.xlsx
+++ b/Project walkthrough.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>PROBLEMS</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Create a Test circuit for infra reciever</t>
+  </si>
+  <si>
+    <t>Parts fits to the box, not fixed yet</t>
   </si>
 </sst>
 </file>
@@ -835,7 +838,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +847,7 @@
     <col min="3" max="3" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -892,8 +895,9 @@
       <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F5" s="10">
         <v>43224</v>
       </c>
@@ -975,13 +979,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="SOLVED">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="SOLVED">
       <formula>NOT(ISERROR(SEARCH("SOLVED",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WORK">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WORK">
       <formula>NOT(ISERROR(SEARCH("WORK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1009,7 +1013,7 @@
     <col min="3" max="3" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1122,13 +1126,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SOLVED">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="SOLVED">
       <formula>NOT(ISERROR(SEARCH("SOLVED",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WORK">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WORK">
       <formula>NOT(ISERROR(SEARCH("WORK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1169,13 +1173,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="SOLVED">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SOLVED">
       <formula>NOT(ISERROR(SEARCH("SOLVED",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WORK">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WORK">
       <formula>NOT(ISERROR(SEARCH("WORK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>